<commit_message>
updated log and work hours
</commit_message>
<xml_diff>
--- a/Notes and Record Files/Jin Li Work Hours.xlsx
+++ b/Notes and Record Files/Jin Li Work Hours.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t xml:space="preserve">Time In </t>
   </si>
@@ -179,6 +179,60 @@
   </si>
   <si>
     <t>looked at hyesun's link to dynamic plotting and added onto graphing ideas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented pretrained word embedding </t>
+  </si>
+  <si>
+    <t>created bar graphs in python for showing frequencies</t>
+  </si>
+  <si>
+    <t>discussed with ben about the art project</t>
+  </si>
+  <si>
+    <t>created word clouds</t>
+  </si>
+  <si>
+    <t>was able to group words together and create bar graphs and scatterplots based on the group</t>
+  </si>
+  <si>
+    <t>added on to log</t>
+  </si>
+  <si>
+    <t>looked and responded to emails</t>
+  </si>
+  <si>
+    <t>skyped with Ben and Michal about our general direction of art analysis</t>
+  </si>
+  <si>
+    <t>looked through Andrew Gelman's book and blog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">researched different sorting algorithms and resources that we might need for the art project </t>
+  </si>
+  <si>
+    <t xml:space="preserve">set up google cloud datalab on my account </t>
+  </si>
+  <si>
+    <t>helped Ben set up too</t>
+  </si>
+  <si>
+    <t>brief visualization on the dataset</t>
+  </si>
+  <si>
+    <t>wrote script to remove corrupted files</t>
+  </si>
+  <si>
+    <t>Wrote a brief script that extracts the style layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">researched types of artistic styles </t>
+  </si>
+  <si>
+    <t>trained a mini batch kmeans algorithm</t>
+  </si>
+  <si>
+    <t>looked into different online training resources</t>
   </si>
 </sst>
 </file>
@@ -1218,6 +1272,21 @@
       <c r="A91" s="1">
         <v>43463.0</v>
       </c>
+      <c r="B91" s="3">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C91" s="3">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="D91" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1">
@@ -1238,68 +1307,238 @@
       <c r="A95" s="1">
         <v>43467.0</v>
       </c>
+      <c r="B95" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C95" s="3">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1">
         <v>43468.0</v>
       </c>
+      <c r="B96" s="3">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="C96" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D96" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="97">
-      <c r="A97" s="6"/>
+      <c r="A97" s="1">
+        <v>43469.0</v>
+      </c>
+      <c r="B97" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C97" s="3">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="D97" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" s="6"/>
+      <c r="A98" s="1">
+        <v>43470.0</v>
+      </c>
+      <c r="B98" s="3">
+        <v>0.3125</v>
+      </c>
+      <c r="C98" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D98" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" s="6"/>
+      <c r="A99" s="1">
+        <v>43471.0</v>
+      </c>
+      <c r="B99" s="3">
+        <v>0.041666666666666664</v>
+      </c>
+      <c r="C99" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D99" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="6"/>
+      <c r="A100" s="1">
+        <v>43472.0</v>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="6"/>
+      <c r="A101" s="1">
+        <v>43473.0</v>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="6"/>
+      <c r="A102" s="1">
+        <v>43474.0</v>
+      </c>
+      <c r="B102" s="3">
+        <v>0.1875</v>
+      </c>
+      <c r="C102" s="3">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="D102" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="103">
-      <c r="A103" s="6"/>
+      <c r="A103" s="1">
+        <v>43475.0</v>
+      </c>
+      <c r="B103" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C103" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D103" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="104">
-      <c r="A104" s="6"/>
+      <c r="A104" s="1">
+        <v>43476.0</v>
+      </c>
+      <c r="B104" s="3">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="C104" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D104" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="105">
-      <c r="A105" s="6"/>
+      <c r="A105" s="1">
+        <v>43477.0</v>
+      </c>
+      <c r="B105" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C105" s="3">
+        <v>0.041666666666666664</v>
+      </c>
+      <c r="D105" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="106">
-      <c r="A106" s="6"/>
+      <c r="A106" s="1">
+        <v>43478.0</v>
+      </c>
     </row>
     <row r="107">
-      <c r="A107" s="6"/>
+      <c r="A107" s="1">
+        <v>43479.0</v>
+      </c>
     </row>
     <row r="108">
-      <c r="A108" s="6"/>
+      <c r="A108" s="1">
+        <v>43480.0</v>
+      </c>
     </row>
     <row r="109">
-      <c r="A109" s="6"/>
+      <c r="A109" s="1">
+        <v>43481.0</v>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" s="6"/>
+      <c r="A110" s="1">
+        <v>43482.0</v>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" s="6"/>
+      <c r="A111" s="1">
+        <v>43483.0</v>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" s="6"/>
+      <c r="A112" s="1">
+        <v>43484.0</v>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" s="6"/>
+      <c r="A113" s="1">
+        <v>43485.0</v>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="6"/>
+      <c r="A114" s="1">
+        <v>43486.0</v>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" s="6"/>
+      <c r="A115" s="1">
+        <v>43487.0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="6"/>

</xml_diff>